<commit_message>
Se agrego Gen Maturin, estamos viendo conectar Gen en paralelo
</commit_message>
<xml_diff>
--- a/Salida/Resultado.xlsx
+++ b/Salida/Resultado.xlsx
@@ -15,16 +15,13 @@
     <sheet name="POWER FLOW GS" sheetId="6" r:id="rId6"/>
     <sheet name="RESULTS NR" sheetId="7" r:id="rId7"/>
     <sheet name="POWER FLOW NR" sheetId="8" r:id="rId8"/>
-    <sheet name="RESULTS DC" sheetId="9" r:id="rId9"/>
-    <sheet name="RESULTS FD" sheetId="10" r:id="rId10"/>
-    <sheet name="POWER FLOW FD" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="63">
   <si>
     <t>STATUS</t>
   </si>
@@ -53,6 +50,12 @@
     <t>Line 1</t>
   </si>
   <si>
+    <t>Line 2</t>
+  </si>
+  <si>
+    <t>Line 3</t>
+  </si>
+  <si>
     <t>Bus type</t>
   </si>
   <si>
@@ -83,21 +86,33 @@
     <t>%P</t>
   </si>
   <si>
-    <t>Bus 1</t>
-  </si>
-  <si>
-    <t>Bus 2</t>
+    <t>Barra 1</t>
+  </si>
+  <si>
+    <t>Barra 2</t>
   </si>
   <si>
     <t>Bolivar</t>
   </si>
   <si>
+    <t>Barra 4</t>
+  </si>
+  <si>
+    <t>Maturin</t>
+  </si>
+  <si>
+    <t>Barra 6</t>
+  </si>
+  <si>
     <t>SL</t>
   </si>
   <si>
     <t>PQ</t>
   </si>
   <si>
+    <t>PV</t>
+  </si>
+  <si>
     <t>Xcc (pu)</t>
   </si>
   <si>
@@ -122,6 +137,21 @@
     <t>TRX 5</t>
   </si>
   <si>
+    <t>TRX 6</t>
+  </si>
+  <si>
+    <t>TRX 7</t>
+  </si>
+  <si>
+    <t>TRX 8</t>
+  </si>
+  <si>
+    <t>TRX 9</t>
+  </si>
+  <si>
+    <t>TRX 10</t>
+  </si>
+  <si>
     <t>X (pu)</t>
   </si>
   <si>
@@ -180,12 +210,6 @@
   </si>
   <si>
     <t>Qji (pu)</t>
-  </si>
-  <si>
-    <t>&lt;V (degree)</t>
-  </si>
-  <si>
-    <t>Indent.</t>
   </si>
 </sst>
 </file>
@@ -543,7 +567,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -595,363 +619,50 @@
         <v>0</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1">
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1">
-        <v>6.090058774901874E-06</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="E3">
+        <v>0.005146875</v>
+      </c>
+      <c r="F3">
+        <v>0.06797250000000001</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3">
-        <v>1.05</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>1.3945</v>
-      </c>
-      <c r="E3">
-        <v>1.1459</v>
-      </c>
-      <c r="F3">
-        <v>1.3945</v>
-      </c>
-      <c r="G3">
-        <v>1.1459</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4">
-        <v>1.0264</v>
-      </c>
       <c r="C4">
-        <v>-1.6313</v>
+        <v>2</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.005146875</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>0.06797250000000001</v>
       </c>
       <c r="G4">
         <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5">
-        <v>1.012</v>
-      </c>
-      <c r="C5">
-        <v>-2.5421</v>
-      </c>
-      <c r="D5">
-        <v>-1.3915</v>
-      </c>
-      <c r="E5">
-        <v>-1.0437</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1.3915</v>
-      </c>
-      <c r="I5">
-        <v>1.0437</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>0.2789</v>
-      </c>
-      <c r="E2">
-        <v>0.2292</v>
-      </c>
-      <c r="F2">
-        <v>-0.2789</v>
-      </c>
-      <c r="G2">
-        <v>-0.2162</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0.01299999999999998</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>0.2789</v>
-      </c>
-      <c r="E3">
-        <v>0.2292</v>
-      </c>
-      <c r="F3">
-        <v>-0.2789</v>
-      </c>
-      <c r="G3">
-        <v>-0.2162</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0.01299999999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>0.2789</v>
-      </c>
-      <c r="E4">
-        <v>0.2292</v>
-      </c>
-      <c r="F4">
-        <v>-0.2789</v>
-      </c>
-      <c r="G4">
-        <v>-0.2162</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0.01299999999999998</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>0.2789</v>
-      </c>
-      <c r="E5">
-        <v>0.2292</v>
-      </c>
-      <c r="F5">
-        <v>-0.2789</v>
-      </c>
-      <c r="G5">
-        <v>-0.2162</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0.01299999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6">
-        <v>0.2789</v>
-      </c>
-      <c r="E6">
-        <v>0.2292</v>
-      </c>
-      <c r="F6">
-        <v>-0.2789</v>
-      </c>
-      <c r="G6">
-        <v>-0.2162</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>0.01299999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>1.3936</v>
-      </c>
-      <c r="E7">
-        <v>1.0812</v>
-      </c>
-      <c r="F7">
-        <v>-1.3908</v>
-      </c>
-      <c r="G7">
-        <v>-1.044</v>
-      </c>
-      <c r="H7">
-        <v>0.002799999999999914</v>
-      </c>
-      <c r="I7">
-        <v>0.0371999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -961,7 +672,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -978,34 +689,34 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1013,13 +724,13 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>1.05</v>
@@ -1054,13 +765,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1095,13 +806,13 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1129,6 +840,129 @@
       </c>
       <c r="M4">
         <v>0.35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>4.5</v>
+      </c>
+      <c r="J6">
+        <v>2.17</v>
+      </c>
+      <c r="K6">
+        <v>0.05</v>
+      </c>
+      <c r="L6">
+        <v>0.05</v>
+      </c>
+      <c r="M6">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1138,7 +972,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1158,13 +992,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1172,7 +1006,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1195,7 +1029,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1218,7 +1052,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1241,7 +1075,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1264,7 +1098,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1280,6 +1114,121 @@
       </c>
       <c r="G6">
         <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>0.1004158790170132</v>
+      </c>
+      <c r="F7">
+        <v>1.02</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>0.1004158790170132</v>
+      </c>
+      <c r="F8">
+        <v>1.02</v>
+      </c>
+      <c r="G8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>0.1004158790170132</v>
+      </c>
+      <c r="F9">
+        <v>1.02</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>0.1002666666666667</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>0.1002666666666667</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1309,7 +1258,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1319,7 +1268,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1327,16 +1276,16 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B1">
         <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D1">
-        <v>9.892829782432674E-05</v>
+        <v>0.002953978739976974</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1344,33 +1293,33 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>1.05</v>
@@ -1379,16 +1328,16 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1.7627</v>
+        <v>-2.5496</v>
       </c>
       <c r="E3">
-        <v>1.4852</v>
+        <v>2.459</v>
       </c>
       <c r="F3">
-        <v>1.7627</v>
+        <v>-2.5496</v>
       </c>
       <c r="G3">
-        <v>1.4852</v>
+        <v>2.459</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1399,13 +1348,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>1.0196</v>
+        <v>0.9999</v>
       </c>
       <c r="C4">
-        <v>-2.0759</v>
+        <v>3.0625</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1428,19 +1377,19 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>1.001</v>
+        <v>0.9912</v>
       </c>
       <c r="C5">
-        <v>-3.2519</v>
+        <v>2.4979</v>
       </c>
       <c r="D5">
-        <v>-1.7643</v>
+        <v>-0.8162</v>
       </c>
       <c r="E5">
-        <v>-1.3233</v>
+        <v>-0.6121</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1449,10 +1398,97 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1.7643</v>
+        <v>0.8162</v>
       </c>
       <c r="I5">
-        <v>1.3233</v>
+        <v>0.6121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>0.9628</v>
+      </c>
+      <c r="C6">
+        <v>10.4066</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>0.9152</v>
+      </c>
+      <c r="C7">
+        <v>18.1556</v>
+      </c>
+      <c r="D7">
+        <v>-2.2945</v>
+      </c>
+      <c r="E7">
+        <v>-1.1065</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>2.2945</v>
+      </c>
+      <c r="I7">
+        <v>1.1065</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>37.3175</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2.7031</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>2.7031</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1462,7 +1498,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1470,7 +1506,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1479,27 +1515,27 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1508,27 +1544,27 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>0.3525</v>
+        <v>-0.5099</v>
       </c>
       <c r="E2">
-        <v>0.297</v>
+        <v>0.4918</v>
       </c>
       <c r="F2">
-        <v>-0.3525</v>
+        <v>0.5099</v>
       </c>
       <c r="G2">
-        <v>-0.2758</v>
+        <v>-0.4417</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.0212</v>
+        <v>0.0501</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1537,27 +1573,27 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>0.3525</v>
+        <v>-0.5099</v>
       </c>
       <c r="E3">
-        <v>0.297</v>
+        <v>0.4918</v>
       </c>
       <c r="F3">
-        <v>-0.3525</v>
+        <v>0.5099</v>
       </c>
       <c r="G3">
-        <v>-0.2758</v>
+        <v>-0.4417</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0.0212</v>
+        <v>0.0501</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1566,27 +1602,27 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>0.3525</v>
+        <v>-0.5099</v>
       </c>
       <c r="E4">
-        <v>0.297</v>
+        <v>0.4918</v>
       </c>
       <c r="F4">
-        <v>-0.3525</v>
+        <v>0.5099</v>
       </c>
       <c r="G4">
-        <v>-0.2758</v>
+        <v>-0.4417</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0.0212</v>
+        <v>0.0501</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1595,27 +1631,27 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>0.3525</v>
+        <v>-0.5099</v>
       </c>
       <c r="E5">
-        <v>0.297</v>
+        <v>0.4918</v>
       </c>
       <c r="F5">
-        <v>-0.3525</v>
+        <v>0.5099</v>
       </c>
       <c r="G5">
-        <v>-0.2758</v>
+        <v>-0.4417</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0.0212</v>
+        <v>0.0501</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1624,22 +1660,22 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>0.3525</v>
+        <v>-0.5099</v>
       </c>
       <c r="E6">
-        <v>0.297</v>
+        <v>0.4918</v>
       </c>
       <c r="F6">
-        <v>-0.3525</v>
+        <v>0.5099</v>
       </c>
       <c r="G6">
-        <v>-0.2758</v>
+        <v>-0.4417</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0.0212</v>
+        <v>0.0501</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1653,22 +1689,225 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>1.7689</v>
+        <v>0.8239</v>
       </c>
       <c r="E7">
-        <v>1.3842</v>
+        <v>0.6319</v>
       </c>
       <c r="F7">
-        <v>-1.7643</v>
+        <v>-0.8228</v>
       </c>
       <c r="G7">
-        <v>-1.3231</v>
+        <v>-0.6183999999999999</v>
       </c>
       <c r="H7">
-        <v>0.0046</v>
+        <v>0.0011</v>
       </c>
       <c r="I7">
-        <v>0.0611</v>
+        <v>0.0135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>-1.7504</v>
+      </c>
+      <c r="E8">
+        <v>0.794</v>
+      </c>
+      <c r="F8">
+        <v>1.7694</v>
+      </c>
+      <c r="G8">
+        <v>-0.5427999999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.019</v>
+      </c>
+      <c r="I8">
+        <v>0.2512</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>-1.7504</v>
+      </c>
+      <c r="E9">
+        <v>0.794</v>
+      </c>
+      <c r="F9">
+        <v>1.7694</v>
+      </c>
+      <c r="G9">
+        <v>-0.5427999999999999</v>
+      </c>
+      <c r="H9">
+        <v>0.019</v>
+      </c>
+      <c r="I9">
+        <v>0.2512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>-1.231</v>
+      </c>
+      <c r="E10">
+        <v>0.3704</v>
+      </c>
+      <c r="F10">
+        <v>1.231</v>
+      </c>
+      <c r="G10">
+        <v>-0.1949</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0.1755</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>-1.231</v>
+      </c>
+      <c r="E11">
+        <v>0.3704</v>
+      </c>
+      <c r="F11">
+        <v>1.231</v>
+      </c>
+      <c r="G11">
+        <v>-0.1949</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0.1755</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>-1.231</v>
+      </c>
+      <c r="E12">
+        <v>0.3704</v>
+      </c>
+      <c r="F12">
+        <v>1.231</v>
+      </c>
+      <c r="G12">
+        <v>-0.1949</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0.1755</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>-2.996</v>
+      </c>
+      <c r="E13">
+        <v>-0.2684</v>
+      </c>
+      <c r="F13">
+        <v>2.996</v>
+      </c>
+      <c r="G13">
+        <v>1.3516</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1.0832</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>-2.996</v>
+      </c>
+      <c r="E14">
+        <v>-0.2684</v>
+      </c>
+      <c r="F14">
+        <v>2.996</v>
+      </c>
+      <c r="G14">
+        <v>1.3516</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1.0832</v>
       </c>
     </row>
   </sheetData>
@@ -1678,7 +1917,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1686,16 +1925,16 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B1">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="D1">
-        <v>9.724753077691023E-05</v>
+        <v>0.002820086199011307</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1703,33 +1942,33 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3">
         <v>1.05</v>
@@ -1738,16 +1977,16 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1.7471</v>
+        <v>-2.9157</v>
       </c>
       <c r="E3">
-        <v>1.4704</v>
+        <v>2.513</v>
       </c>
       <c r="F3">
-        <v>1.7471</v>
+        <v>-2.9157</v>
       </c>
       <c r="G3">
-        <v>1.4704</v>
+        <v>2.513</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1758,13 +1997,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>1.0198</v>
+        <v>0.9992</v>
       </c>
       <c r="C4">
-        <v>-2.057</v>
+        <v>3.5051</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1787,19 +2026,19 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B5">
-        <v>1.0016</v>
+        <v>0.9912</v>
       </c>
       <c r="C5">
-        <v>-3.2176</v>
+        <v>2.9803</v>
       </c>
       <c r="D5">
-        <v>-1.7454</v>
+        <v>-0.7573</v>
       </c>
       <c r="E5">
-        <v>-1.3091</v>
+        <v>-0.5679999999999999</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -1808,10 +2047,97 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>1.7454</v>
+        <v>0.7573</v>
       </c>
       <c r="I5">
-        <v>1.3091</v>
+        <v>0.5679999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>0.9617</v>
+      </c>
+      <c r="C6">
+        <v>11.2349</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>0.9144</v>
+      </c>
+      <c r="C7">
+        <v>19.2121</v>
+      </c>
+      <c r="D7">
+        <v>-2.2495</v>
+      </c>
+      <c r="E7">
+        <v>-1.0848</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>2.2495</v>
+      </c>
+      <c r="I7">
+        <v>1.0848</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>38.4244</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>2.724</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>2.724</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1821,7 +2147,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1829,7 +2155,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1838,22 +2164,22 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1867,27 +2193,27 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>0.3494</v>
+        <v>-0.5831</v>
       </c>
       <c r="E2">
-        <v>0.2941</v>
+        <v>0.5026</v>
       </c>
       <c r="F2">
-        <v>-0.3494</v>
+        <v>0.5831</v>
       </c>
       <c r="G2">
-        <v>-0.2733</v>
+        <v>-0.4435</v>
       </c>
       <c r="H2">
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0.02079999999999999</v>
+        <v>0.05910000000000004</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1896,27 +2222,27 @@
         <v>4</v>
       </c>
       <c r="D3">
-        <v>0.3494</v>
+        <v>-0.5831</v>
       </c>
       <c r="E3">
-        <v>0.2941</v>
+        <v>0.5026</v>
       </c>
       <c r="F3">
-        <v>-0.3494</v>
+        <v>0.5831</v>
       </c>
       <c r="G3">
-        <v>-0.2733</v>
+        <v>-0.4435</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0.02079999999999999</v>
+        <v>0.05910000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1925,27 +2251,27 @@
         <v>2</v>
       </c>
       <c r="D4">
-        <v>0.3494</v>
+        <v>-0.5831</v>
       </c>
       <c r="E4">
-        <v>0.2941</v>
+        <v>0.5026</v>
       </c>
       <c r="F4">
-        <v>-0.3494</v>
+        <v>0.5831</v>
       </c>
       <c r="G4">
-        <v>-0.2733</v>
+        <v>-0.4435</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0.02079999999999999</v>
+        <v>0.05910000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1954,27 +2280,27 @@
         <v>2</v>
       </c>
       <c r="D5">
-        <v>0.3494</v>
+        <v>-0.5831</v>
       </c>
       <c r="E5">
-        <v>0.2941</v>
+        <v>0.5026</v>
       </c>
       <c r="F5">
-        <v>-0.3494</v>
+        <v>0.5831</v>
       </c>
       <c r="G5">
-        <v>-0.2733</v>
+        <v>-0.4435</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0.02079999999999999</v>
+        <v>0.05910000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1983,22 +2309,22 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>0.3494</v>
+        <v>-0.5831</v>
       </c>
       <c r="E6">
-        <v>0.2941</v>
+        <v>0.5026</v>
       </c>
       <c r="F6">
-        <v>-0.3494</v>
+        <v>0.5831</v>
       </c>
       <c r="G6">
-        <v>-0.2733</v>
+        <v>-0.4435</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0.02079999999999999</v>
+        <v>0.05910000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2012,67 +2338,225 @@
         <v>3</v>
       </c>
       <c r="D7">
-        <v>1.747</v>
+        <v>0.765</v>
       </c>
       <c r="E7">
-        <v>1.3664</v>
+        <v>0.5849</v>
       </c>
       <c r="F7">
-        <v>-1.7425</v>
+        <v>-0.7641</v>
       </c>
       <c r="G7">
-        <v>-1.3069</v>
+        <v>-0.5732</v>
       </c>
       <c r="H7">
-        <v>0.004500000000000171</v>
+        <v>0.0009000000000000119</v>
       </c>
       <c r="I7">
-        <v>0.05950000000000011</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>-8.663121862378047</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>-9.660068425905679</v>
+        <v>0.01169999999999993</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>-1.8395</v>
+      </c>
+      <c r="E8">
+        <v>0.8191000000000001</v>
+      </c>
+      <c r="F8">
+        <v>1.8604</v>
+      </c>
+      <c r="G8">
+        <v>-0.5431</v>
+      </c>
+      <c r="H8">
+        <v>0.02090000000000014</v>
+      </c>
+      <c r="I8">
+        <v>0.276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>-1.8395</v>
+      </c>
+      <c r="E9">
+        <v>0.8191000000000001</v>
+      </c>
+      <c r="F9">
+        <v>1.8604</v>
+      </c>
+      <c r="G9">
+        <v>-0.5431</v>
+      </c>
+      <c r="H9">
+        <v>0.02090000000000014</v>
+      </c>
+      <c r="I9">
+        <v>0.276</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>-1.2644</v>
+      </c>
+      <c r="E10">
+        <v>0.3721</v>
+      </c>
+      <c r="F10">
+        <v>1.2644</v>
+      </c>
+      <c r="G10">
+        <v>-0.1872</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0.1849</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>-1.2644</v>
+      </c>
+      <c r="E11">
+        <v>0.3721</v>
+      </c>
+      <c r="F11">
+        <v>1.2644</v>
+      </c>
+      <c r="G11">
+        <v>-0.1872</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0.1849</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>-1.2644</v>
+      </c>
+      <c r="E12">
+        <v>0.3721</v>
+      </c>
+      <c r="F12">
+        <v>1.2644</v>
+      </c>
+      <c r="G12">
+        <v>-0.1872</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0.1849</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>-3.0009</v>
+      </c>
+      <c r="E13">
+        <v>-0.2731</v>
+      </c>
+      <c r="F13">
+        <v>3.0009</v>
+      </c>
+      <c r="G13">
+        <v>1.362</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1.0889</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>-3.0009</v>
+      </c>
+      <c r="E14">
+        <v>-0.2731</v>
+      </c>
+      <c r="F14">
+        <v>3.0009</v>
+      </c>
+      <c r="G14">
+        <v>1.362</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1.0889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>